<commit_message>
cambio de archivo .env
</commit_message>
<xml_diff>
--- a/temp/SERVICIOS 2025.xlsx
+++ b/temp/SERVICIOS 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481498B3C4373867/DOCUMENTOS_EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2578" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CDA4F68-BB81-4FE5-AEDB-F6B483EC049E}"/>
+  <xr:revisionPtr revIDLastSave="2586" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F790C3A8-7746-9B46-9B0D-E3B224C3EDF2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="8" xr2:uid="{58C13FB9-58C5-4D53-86A7-FA1AAB49DCCE}"/>
   </bookViews>
@@ -26,10 +26,21 @@
     <sheet name="NOVIEMBRE" sheetId="11" r:id="rId11"/>
     <sheet name="DICIEMBRE" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -39,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="674">
   <si>
     <t>FECHA</t>
   </si>
@@ -2052,6 +2063,15 @@
   </si>
   <si>
     <t>JG  hace transferencia de $185.600 para copletar el pago del servicio a ABRECAR el cliente ya le habia abonado $450.000 este pago incluye los $60.000 de la bateria y la caja que se tomaron de la oficina y los $40.000 de la visita inicial se hizo por transferencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALLE 23 SUR # 6 - 31 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yamcar Carlos Díaz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajuste de puertas de vidrio corredizas entrada y chapa mantenimiento </t>
   </si>
 </sst>
 </file>
@@ -2217,40 +2237,75 @@
   </cellStyles>
   <dxfs count="546">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2273,16 +2328,75 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2609,7 +2723,10 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -2664,19 +2781,30 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2704,136 +2832,28 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -4744,7 +4764,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3DC7B56-6A27-47EA-8A62-6146CB27CD41}" name="Tabla14567891011" displayName="Tabla14567891011" ref="A1:S41" totalsRowCount="1" headerRowDxfId="121" dataDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3DC7B56-6A27-47EA-8A62-6146CB27CD41}" name="Tabla14567891011" displayName="Tabla14567891011" ref="A1:S41" totalsRowCount="1" headerRowDxfId="104" dataDxfId="103">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4767,38 +4787,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{94F08EE5-D270-4BBA-BFF0-760C6EE7067B}" name="FECHA" totalsRowLabel="Total" dataDxfId="119" totalsRowDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{4C53B68C-163E-46DC-B529-42A48BCB11F4}" name="DIRECCION" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{79BD3134-74F1-4163-BEA0-1250C669D816}" name="NOMBRE CLIENTE" dataDxfId="116"/>
-    <tableColumn id="4" xr3:uid="{9B7351AF-69A8-42A0-88CF-7F1D324558CD}" name="TORRE/APTO" dataDxfId="115"/>
-    <tableColumn id="5" xr3:uid="{3FC795B0-64D5-412F-967D-88FDCE6188CC}" name="SERVICIO REALIZADO" dataDxfId="114"/>
-    <tableColumn id="6" xr3:uid="{F8E4C084-C1E1-410A-9AB8-48E3E1C03449}" name="DOMICILIO" dataDxfId="113" totalsRowDxfId="112" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{3923866B-5E04-4E69-B31A-D524F1DB0AAC}" name="VALOR SERVICIO" dataDxfId="111" totalsRowDxfId="110"/>
-    <tableColumn id="8" xr3:uid="{8D9C03FA-D5F4-4C9D-B0D6-0B3FE724EB6D}" name="MATERIALES" dataDxfId="109"/>
-    <tableColumn id="9" xr3:uid="{416A2E87-138A-49CF-B9F5-D318A063AD9F}" name="VALOR MATERIALES" dataDxfId="108"/>
-    <tableColumn id="10" xr3:uid="{A82F5C41-8889-4BC2-8CD0-E17F28FC8B69}" name="IVA 19%" dataDxfId="107"/>
-    <tableColumn id="11" xr3:uid="{8AE9AA77-4CCE-4933-9E37-2424517466ED}" name="PORTERIA" dataDxfId="106" totalsRowDxfId="105"/>
-    <tableColumn id="12" xr3:uid="{9AEF8C4D-8BF9-4E7D-B1C4-77744EC693C7}" name="FORMA DE PAGO " dataDxfId="104"/>
-    <tableColumn id="13" xr3:uid="{E6A473EB-A02F-4383-8D91-3F21721D15F3}" name="TOTAL SERVICIO" dataDxfId="103" totalsRowDxfId="102">
+    <tableColumn id="1" xr3:uid="{94F08EE5-D270-4BBA-BFF0-760C6EE7067B}" name="FECHA" totalsRowLabel="Total" dataDxfId="102" totalsRowDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{4C53B68C-163E-46DC-B529-42A48BCB11F4}" name="DIRECCION" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{79BD3134-74F1-4163-BEA0-1250C669D816}" name="NOMBRE CLIENTE" dataDxfId="99"/>
+    <tableColumn id="4" xr3:uid="{9B7351AF-69A8-42A0-88CF-7F1D324558CD}" name="TORRE/APTO" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{3FC795B0-64D5-412F-967D-88FDCE6188CC}" name="SERVICIO REALIZADO" dataDxfId="97"/>
+    <tableColumn id="6" xr3:uid="{F8E4C084-C1E1-410A-9AB8-48E3E1C03449}" name="DOMICILIO" dataDxfId="96" totalsRowDxfId="95" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{3923866B-5E04-4E69-B31A-D524F1DB0AAC}" name="VALOR SERVICIO" dataDxfId="94" totalsRowDxfId="93"/>
+    <tableColumn id="8" xr3:uid="{8D9C03FA-D5F4-4C9D-B0D6-0B3FE724EB6D}" name="MATERIALES" dataDxfId="92"/>
+    <tableColumn id="9" xr3:uid="{416A2E87-138A-49CF-B9F5-D318A063AD9F}" name="VALOR MATERIALES" dataDxfId="91"/>
+    <tableColumn id="10" xr3:uid="{A82F5C41-8889-4BC2-8CD0-E17F28FC8B69}" name="IVA 19%" dataDxfId="90"/>
+    <tableColumn id="11" xr3:uid="{8AE9AA77-4CCE-4933-9E37-2424517466ED}" name="PORTERIA" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{9AEF8C4D-8BF9-4E7D-B1C4-77744EC693C7}" name="FORMA DE PAGO " dataDxfId="87"/>
+    <tableColumn id="13" xr3:uid="{E6A473EB-A02F-4383-8D91-3F21721D15F3}" name="TOTAL SERVICIO" dataDxfId="86" totalsRowDxfId="85">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{D278A045-9615-406B-B68A-49A1BAA68123}" name="X50%/X25%" dataDxfId="101" totalsRowDxfId="100"/>
-    <tableColumn id="15" xr3:uid="{27DD6F2B-55CE-4F91-802C-767D2081AE8F}" name="PARA JG" dataDxfId="99" totalsRowDxfId="98">
+    <tableColumn id="14" xr3:uid="{D278A045-9615-406B-B68A-49A1BAA68123}" name="X50%/X25%" dataDxfId="84" totalsRowDxfId="83"/>
+    <tableColumn id="15" xr3:uid="{27DD6F2B-55CE-4F91-802C-767D2081AE8F}" name="PARA JG" dataDxfId="82" totalsRowDxfId="81">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{A3F60C5A-D316-497E-B0E4-A3F9BAD84525}" name="PARA ABRECAR" dataDxfId="97" totalsRowDxfId="96">
+    <tableColumn id="16" xr3:uid="{A3F60C5A-D316-497E-B0E4-A3F9BAD84525}" name="PARA ABRECAR" dataDxfId="80" totalsRowDxfId="79">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{10CB3E58-1A46-4C24-BA4F-AC5B36B8FF91}" name="ESTADO DEL SERVICIO" dataDxfId="95" totalsRowDxfId="94"/>
-    <tableColumn id="18" xr3:uid="{8BFE1AAE-4E74-4C50-BDE1-0DB10D889E57}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="19" xr3:uid="{206EECE6-638F-4588-8E77-382586BB3883}" name="NOTAS " totalsRowFunction="count" dataDxfId="91"/>
+    <tableColumn id="17" xr3:uid="{10CB3E58-1A46-4C24-BA4F-AC5B36B8FF91}" name="ESTADO DEL SERVICIO" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="18" xr3:uid="{8BFE1AAE-4E74-4C50-BDE1-0DB10D889E57}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="19" xr3:uid="{206EECE6-638F-4588-8E77-382586BB3883}" name="NOTAS " totalsRowFunction="count" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{DDAE932D-094A-412C-ACB3-D50B4144C427}" name="Tabla1456789101112" displayName="Tabla1456789101112" ref="A1:S41" totalsRowCount="1" headerRowDxfId="84" dataDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{DDAE932D-094A-412C-ACB3-D50B4144C427}" name="Tabla1456789101112" displayName="Tabla1456789101112" ref="A1:S41" totalsRowCount="1" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4821,38 +4841,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{A4610472-FCCC-49A0-A01F-092A0D751A98}" name="FECHA" totalsRowLabel="Total" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{F9E90005-75E9-4DFD-BEDF-137ACD9E05E4}" name="DIRECCION" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{F27B45B3-7483-405C-8490-165648DB5719}" name="NOMBRE CLIENTE" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{0FACF2B2-755C-4F0C-BA8A-14DC07017FD9}" name="TORRE/APTO" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{00E06524-BE36-4FF3-976B-47960F284CE0}" name="SERVICIO REALIZADO" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{5E93EC92-00AD-4B71-80D9-5F0B68DA5499}" name="DOMICILIO" dataDxfId="76" totalsRowDxfId="75" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FF6104F0-B72E-428D-8D64-20449974A374}" name="VALOR SERVICIO" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{CBA086A4-170D-485A-BDFD-EA146BD0B019}" name="MATERIALES" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{21A2EE02-A6EA-4899-886D-AFD1BA8755C3}" name="VALOR MATERIALES" dataDxfId="71"/>
-    <tableColumn id="10" xr3:uid="{1D00EAAB-65B1-4167-A677-7DFEA1816D65}" name="IVA 19%" dataDxfId="70"/>
-    <tableColumn id="11" xr3:uid="{2009E649-7D60-4DDB-8525-08B12BD6FA59}" name="PORTERIA" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="12" xr3:uid="{54BC3D94-5458-4653-8053-00D38144E7B3}" name="FORMA DE PAGO " dataDxfId="67"/>
-    <tableColumn id="13" xr3:uid="{A1498961-0B31-4EC8-87A8-0CA896C0FA28}" name="TOTAL SERVICIO" dataDxfId="66" totalsRowDxfId="65">
+    <tableColumn id="1" xr3:uid="{A4610472-FCCC-49A0-A01F-092A0D751A98}" name="FECHA" totalsRowLabel="Total" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{F9E90005-75E9-4DFD-BEDF-137ACD9E05E4}" name="DIRECCION" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{F27B45B3-7483-405C-8490-165648DB5719}" name="NOMBRE CLIENTE" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{0FACF2B2-755C-4F0C-BA8A-14DC07017FD9}" name="TORRE/APTO" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{00E06524-BE36-4FF3-976B-47960F284CE0}" name="SERVICIO REALIZADO" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{5E93EC92-00AD-4B71-80D9-5F0B68DA5499}" name="DOMICILIO" dataDxfId="59" totalsRowDxfId="58" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF6104F0-B72E-428D-8D64-20449974A374}" name="VALOR SERVICIO" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{CBA086A4-170D-485A-BDFD-EA146BD0B019}" name="MATERIALES" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{21A2EE02-A6EA-4899-886D-AFD1BA8755C3}" name="VALOR MATERIALES" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{1D00EAAB-65B1-4167-A677-7DFEA1816D65}" name="IVA 19%" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{2009E649-7D60-4DDB-8525-08B12BD6FA59}" name="PORTERIA" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{54BC3D94-5458-4653-8053-00D38144E7B3}" name="FORMA DE PAGO " dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{A1498961-0B31-4EC8-87A8-0CA896C0FA28}" name="TOTAL SERVICIO" dataDxfId="49" totalsRowDxfId="48">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DCA18CC6-6586-4991-B645-0EFDB3C671BA}" name="X50%/X25%" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="15" xr3:uid="{EBD3F72E-644C-4987-97C9-741E83FF57A3}" name="PARA JG" dataDxfId="62" totalsRowDxfId="61">
+    <tableColumn id="14" xr3:uid="{DCA18CC6-6586-4991-B645-0EFDB3C671BA}" name="X50%/X25%" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="15" xr3:uid="{EBD3F72E-644C-4987-97C9-741E83FF57A3}" name="PARA JG" dataDxfId="45" totalsRowDxfId="44">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{582650E7-2FDF-4443-B176-6BD13705FC6A}" name="PARA ABRECAR" dataDxfId="60" totalsRowDxfId="59">
+    <tableColumn id="16" xr3:uid="{582650E7-2FDF-4443-B176-6BD13705FC6A}" name="PARA ABRECAR" dataDxfId="43" totalsRowDxfId="42">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{C9C0844F-A579-409B-A3CA-4CABDCA9A7E7}" name="ESTADO DEL SERVICIO" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="18" xr3:uid="{9BE8DE12-7A02-496D-8A4C-CF6A0FC21298}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="19" xr3:uid="{D05F4CC4-F427-42DD-B60E-F5C5874B0A10}" name="NOTAS " totalsRowFunction="count" dataDxfId="54"/>
+    <tableColumn id="17" xr3:uid="{C9C0844F-A579-409B-A3CA-4CABDCA9A7E7}" name="ESTADO DEL SERVICIO" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="18" xr3:uid="{9BE8DE12-7A02-496D-8A4C-CF6A0FC21298}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="19" xr3:uid="{D05F4CC4-F427-42DD-B60E-F5C5874B0A10}" name="NOTAS " totalsRowFunction="count" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4DF269EC-EC4E-479C-AE4F-1A1087AFCEE8}" name="Tabla145678910111213" displayName="Tabla145678910111213" ref="A1:S41" totalsRowCount="1" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4DF269EC-EC4E-479C-AE4F-1A1087AFCEE8}" name="Tabla145678910111213" displayName="Tabla145678910111213" ref="A1:S41" totalsRowCount="1" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4875,31 +4895,31 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{5055830B-9862-472C-85F0-117E805E707D}" name="FECHA" totalsRowLabel="Total" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{689C0FB3-87A6-4631-B1F6-2F9FCAA7E7B1}" name="DIRECCION" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{C1D134A7-FB44-4236-BBB6-7369A781153D}" name="NOMBRE CLIENTE" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{BD93EBE9-5715-4A8F-8BCE-7ED7B4E1EE00}" name="TORRE/APTO" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{D8732EE5-4B90-470C-AF7D-A9E30BB207AC}" name="SERVICIO REALIZADO" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{AAF6961D-5DCD-413C-8B1C-ACEFB0A3CFD9}" name="DOMICILIO" dataDxfId="39" totalsRowDxfId="38" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{65ABEA60-8C9B-41B7-A56F-8019CBE25FF3}" name="VALOR SERVICIO" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{37401935-4C50-4C18-9EE8-ACDC29848F03}" name="MATERIALES" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{A93E3FC1-DC4F-4F49-A038-306F3DB5A2D6}" name="VALOR MATERIALES" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{D4E56074-FD4E-417D-B429-880CC1DD6054}" name="IVA 19%" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{A07BC7C7-BC63-43A4-A1DF-7229BD46E6AD}" name="PORTERIA" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{2AFC385D-3407-49B7-BF00-60E625E847AA}" name="FORMA DE PAGO " dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{E2603AC2-0F91-4E56-9786-C317F0769BE6}" name="TOTAL SERVICIO" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="1" xr3:uid="{5055830B-9862-472C-85F0-117E805E707D}" name="FECHA" totalsRowLabel="Total" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{689C0FB3-87A6-4631-B1F6-2F9FCAA7E7B1}" name="DIRECCION" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{C1D134A7-FB44-4236-BBB6-7369A781153D}" name="NOMBRE CLIENTE" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{BD93EBE9-5715-4A8F-8BCE-7ED7B4E1EE00}" name="TORRE/APTO" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{D8732EE5-4B90-470C-AF7D-A9E30BB207AC}" name="SERVICIO REALIZADO" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{AAF6961D-5DCD-413C-8B1C-ACEFB0A3CFD9}" name="DOMICILIO" dataDxfId="22" totalsRowDxfId="21" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{65ABEA60-8C9B-41B7-A56F-8019CBE25FF3}" name="VALOR SERVICIO" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{37401935-4C50-4C18-9EE8-ACDC29848F03}" name="MATERIALES" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{A93E3FC1-DC4F-4F49-A038-306F3DB5A2D6}" name="VALOR MATERIALES" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{D4E56074-FD4E-417D-B429-880CC1DD6054}" name="IVA 19%" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{A07BC7C7-BC63-43A4-A1DF-7229BD46E6AD}" name="PORTERIA" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{2AFC385D-3407-49B7-BF00-60E625E847AA}" name="FORMA DE PAGO " dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{E2603AC2-0F91-4E56-9786-C317F0769BE6}" name="TOTAL SERVICIO" dataDxfId="12" totalsRowDxfId="11">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{FD5B7BBF-B716-48D2-B942-472BC782EC98}" name="X50%/X25%" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="15" xr3:uid="{7D676C93-BA72-46B0-9F8A-8787870D86D0}" name="PARA JG" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="14" xr3:uid="{FD5B7BBF-B716-48D2-B942-472BC782EC98}" name="X50%/X25%" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{7D676C93-BA72-46B0-9F8A-8787870D86D0}" name="PARA JG" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{BE3B5891-889F-41B1-B172-6BB026E6D50C}" name="PARA ABRECAR" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="16" xr3:uid="{BE3B5891-889F-41B1-B172-6BB026E6D50C}" name="PARA ABRECAR" dataDxfId="6" totalsRowDxfId="5">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A5F392B8-0A11-4121-9E91-E628125AA82C}" name="ESTADO DEL SERVICIO" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{553C6916-0493-4196-B3C4-4AC2BD6C71D7}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{131F3898-DF9C-4BB0-BA07-9F2E882DFC9F}" name="NOTAS " totalsRowFunction="count" dataDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{A5F392B8-0A11-4121-9E91-E628125AA82C}" name="ESTADO DEL SERVICIO" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{553C6916-0493-4196-B3C4-4AC2BD6C71D7}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{131F3898-DF9C-4BB0-BA07-9F2E882DFC9F}" name="NOTAS " totalsRowFunction="count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5307,31 +5327,31 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C2D31F11-B0BA-45D5-A040-55DD65048FCC}" name="FECHA" totalsRowLabel="Total" dataDxfId="146" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{B04728B5-7F2E-44D9-B119-EB74F66021FF}" name="DIRECCION" dataDxfId="145" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{34B0BF1B-1E1D-4372-8717-57CDDED3EB64}" name="NOMBRE CLIENTE" dataDxfId="144" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{967AF0A4-2F6B-4902-9EE6-06F9B0ACEC7A}" name="TORRE/APTO" dataDxfId="143"/>
-    <tableColumn id="5" xr3:uid="{B7841EF7-1A13-48C8-9A8F-D8ECA1354F32}" name="SERVICIO REALIZADO" dataDxfId="142" totalsRowDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{A5BD60C3-0F5D-4F7B-93D1-EAD5F5FF1B0B}" name="DOMICILIO" dataDxfId="141" totalsRowDxfId="12" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FE128F0E-0F30-41E9-92BC-73866EC54093}" name="VALOR SERVICIO" dataDxfId="140" totalsRowDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{DBFFBE5A-0B3E-47AA-B221-A8BE3A93FA28}" name="MATERIALES" dataDxfId="139" totalsRowDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{E9AB51AF-E4E3-40DA-AB54-3DB3F1C528DD}" name="VALOR MATERIALES" dataDxfId="138" totalsRowDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{0743077C-2C9E-4460-A4B5-D885E65A0FDD}" name="IVA 19%" dataDxfId="137" totalsRowDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{5A1B6F72-1F83-47CD-8CB7-E840972ECC16}" name="PORTERIA" dataDxfId="136" totalsRowDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{85785C1E-0B1B-4AE4-9899-F57CBFBDFCAB}" name="FORMA DE PAGO " dataDxfId="135"/>
-    <tableColumn id="13" xr3:uid="{14E1E447-46F1-4DAB-8DAF-E7F4E090CDF7}" name="TOTAL SERVICIO" dataDxfId="134" totalsRowDxfId="6">
+    <tableColumn id="1" xr3:uid="{C2D31F11-B0BA-45D5-A040-55DD65048FCC}" name="FECHA" totalsRowLabel="Total" dataDxfId="146" totalsRowDxfId="145"/>
+    <tableColumn id="2" xr3:uid="{B04728B5-7F2E-44D9-B119-EB74F66021FF}" name="DIRECCION" dataDxfId="144" totalsRowDxfId="143"/>
+    <tableColumn id="3" xr3:uid="{34B0BF1B-1E1D-4372-8717-57CDDED3EB64}" name="NOMBRE CLIENTE" dataDxfId="142" totalsRowDxfId="141"/>
+    <tableColumn id="4" xr3:uid="{967AF0A4-2F6B-4902-9EE6-06F9B0ACEC7A}" name="TORRE/APTO" dataDxfId="140"/>
+    <tableColumn id="5" xr3:uid="{B7841EF7-1A13-48C8-9A8F-D8ECA1354F32}" name="SERVICIO REALIZADO" dataDxfId="139" totalsRowDxfId="138"/>
+    <tableColumn id="6" xr3:uid="{A5BD60C3-0F5D-4F7B-93D1-EAD5F5FF1B0B}" name="DOMICILIO" dataDxfId="137" totalsRowDxfId="136" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FE128F0E-0F30-41E9-92BC-73866EC54093}" name="VALOR SERVICIO" dataDxfId="135" totalsRowDxfId="134"/>
+    <tableColumn id="8" xr3:uid="{DBFFBE5A-0B3E-47AA-B221-A8BE3A93FA28}" name="MATERIALES" dataDxfId="133" totalsRowDxfId="132"/>
+    <tableColumn id="9" xr3:uid="{E9AB51AF-E4E3-40DA-AB54-3DB3F1C528DD}" name="VALOR MATERIALES" dataDxfId="131" totalsRowDxfId="130"/>
+    <tableColumn id="10" xr3:uid="{0743077C-2C9E-4460-A4B5-D885E65A0FDD}" name="IVA 19%" dataDxfId="129" totalsRowDxfId="128"/>
+    <tableColumn id="11" xr3:uid="{5A1B6F72-1F83-47CD-8CB7-E840972ECC16}" name="PORTERIA" dataDxfId="127" totalsRowDxfId="126"/>
+    <tableColumn id="12" xr3:uid="{85785C1E-0B1B-4AE4-9899-F57CBFBDFCAB}" name="FORMA DE PAGO " dataDxfId="125"/>
+    <tableColumn id="13" xr3:uid="{14E1E447-46F1-4DAB-8DAF-E7F4E090CDF7}" name="TOTAL SERVICIO" dataDxfId="124" totalsRowDxfId="123">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{D122C8FB-7087-4CB5-A785-D8505B2DF602}" name="X50%/X25%" dataDxfId="133" totalsRowDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{3B9C0FF4-0A40-425E-AF56-D6DD8681A011}" name="PARA JG" dataDxfId="132" totalsRowDxfId="4">
+    <tableColumn id="14" xr3:uid="{D122C8FB-7087-4CB5-A785-D8505B2DF602}" name="X50%/X25%" dataDxfId="122" totalsRowDxfId="121"/>
+    <tableColumn id="15" xr3:uid="{3B9C0FF4-0A40-425E-AF56-D6DD8681A011}" name="PARA JG" dataDxfId="120" totalsRowDxfId="119">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{24D7D408-20DD-481D-ADD8-31427D9706CB}" name="PARA ABRECAR" dataDxfId="131" totalsRowDxfId="3">
+    <tableColumn id="16" xr3:uid="{24D7D408-20DD-481D-ADD8-31427D9706CB}" name="PARA ABRECAR" dataDxfId="118" totalsRowDxfId="117">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{3E22CA66-02BA-4F3A-BC78-1C5E81DF6614}" name="ESTADO DEL SERVICIO" dataDxfId="130" totalsRowDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{BC2DF013-F795-4D1C-9028-1375AF4523CB}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="129" totalsRowDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{72057D85-7D90-4121-8CBD-7448786FF9BC}" name="NOTAS " totalsRowFunction="count" dataDxfId="128" totalsRowDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{3E22CA66-02BA-4F3A-BC78-1C5E81DF6614}" name="ESTADO DEL SERVICIO" dataDxfId="116" totalsRowDxfId="115"/>
+    <tableColumn id="18" xr3:uid="{BC2DF013-F795-4D1C-9028-1375AF4523CB}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="114" totalsRowDxfId="113"/>
+    <tableColumn id="19" xr3:uid="{72057D85-7D90-4121-8CBD-7448786FF9BC}" name="NOTAS " totalsRowFunction="count" dataDxfId="112" totalsRowDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8668,22 +8688,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="127" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9977,22 +9997,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="90" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11286,22 +11306,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="53" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23639,8 +23659,8 @@
   </sheetPr>
   <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R11" sqref="R10:R11"/>
+    <sheetView tabSelected="1" topLeftCell="L4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24217,30 +24237,46 @@
         <v>670</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="14"/>
-      <c r="G11" s="17"/>
+    <row r="11" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>45918</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>672</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>673</v>
+      </c>
+      <c r="G11" s="17">
+        <v>180000</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="14"/>
+      <c r="L11" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="M11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="14"/>
-      <c r="O11" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>180000</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="1"/>
+        <v>90000</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="2"/>

</xml_diff>